<commit_message>
Testing download and scripts
</commit_message>
<xml_diff>
--- a/model_results.xlsx
+++ b/model_results.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Kaggle\HIV\Adam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\your_path_here\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="4110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="50670" windowHeight="17820"/>
   </bookViews>
   <sheets>
     <sheet name="model_results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>PatientID</t>
   </si>
@@ -35,15 +35,28 @@
   <si>
     <t>Accuracy</t>
   </si>
+  <si>
+    <t>PASTE DATA BELOW!</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>(All zeroes as a prediction)</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.00000%"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.00000%"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,8 +199,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,8 +395,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -483,6 +517,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -529,10 +589,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="33" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -855,271 +920,281 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K156"/>
+  <dimension ref="A1:L157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B155"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="2">
-        <f>G156</f>
+      <c r="K4" s="2">
+        <f>G157</f>
         <v>0.79470198675496684</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <f>IF(B4=E4,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f>IF(B5=E5,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="D5">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>7</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <f t="shared" ref="G5:G68" si="0">IF(B5=E5,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G69" si="0">IF(B6=E6,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="D6">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>11</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0.79470200000000002</v>
+      </c>
+      <c r="L7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>24</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="D7">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>24</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>29</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="D8">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>29</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="7">
+        <f>K4-K7</f>
+        <v>-1.3245033181341626E-8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>30</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="D9">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="D10">
         <v>30</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>38</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="D10">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="D11">
         <v>38</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>47</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="D11">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="D12">
         <v>47</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>50</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="D12">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="D13">
         <v>50</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>55</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="D13">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="D14">
         <v>55</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>56</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="D14">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="D15">
         <v>56</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>60</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="D15">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="D16">
         <v>60</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>64</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>64</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1131,13 +1206,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1149,13 +1224,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1167,13 +1242,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1185,13 +1260,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1203,13 +1278,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1221,13 +1296,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1239,13 +1314,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1257,13 +1332,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1275,13 +1350,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1293,13 +1368,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1311,13 +1386,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="D27">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1329,13 +1404,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1347,13 +1422,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="D29">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1365,13 +1440,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1383,13 +1458,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="D31">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -1401,13 +1476,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1419,13 +1494,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="D33">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1437,13 +1512,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1455,13 +1530,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1473,13 +1548,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1491,13 +1566,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1509,13 +1584,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1527,13 +1602,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -1545,13 +1620,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -1563,13 +1638,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -1581,13 +1656,13 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -1599,13 +1674,13 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="D43">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -1617,13 +1692,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="D44">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1635,13 +1710,13 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
       <c r="D45">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1653,13 +1728,13 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="D46">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -1671,13 +1746,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
       <c r="D47">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -1689,13 +1764,13 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="D48">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -1707,13 +1782,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
       <c r="D49">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -1725,13 +1800,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="D50">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -1743,13 +1818,13 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="D51">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -1761,13 +1836,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="D52">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -1779,13 +1854,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="D53">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -1797,13 +1872,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B54">
         <v>0</v>
       </c>
       <c r="D54">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -1815,13 +1890,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="D55">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -1833,13 +1908,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
       <c r="D56">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -1851,13 +1926,13 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B57">
         <v>0</v>
       </c>
       <c r="D57">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -1869,13 +1944,13 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B58">
         <v>0</v>
       </c>
       <c r="D58">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -1887,13 +1962,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>348</v>
+        <v>316</v>
       </c>
       <c r="B59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>348</v>
+        <v>316</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -1905,13 +1980,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -1923,13 +1998,13 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>368</v>
+        <v>349</v>
       </c>
       <c r="B61">
         <v>0</v>
       </c>
       <c r="D61">
-        <v>368</v>
+        <v>349</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -1941,13 +2016,13 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="B62">
         <v>0</v>
       </c>
       <c r="D62">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -1959,13 +2034,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -1977,13 +2052,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B64">
         <v>0</v>
       </c>
       <c r="D64">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -1995,13 +2070,13 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B65">
         <v>0</v>
       </c>
       <c r="D65">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -2013,13 +2088,13 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="D66">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -2031,13 +2106,13 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="D67">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -2049,13 +2124,13 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B68">
         <v>0</v>
       </c>
       <c r="D68">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -2067,49 +2142,49 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>441</v>
+        <v>412</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="D69">
-        <v>441</v>
+        <v>412</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
       <c r="G69">
-        <f t="shared" ref="G69:G132" si="1">IF(B69=E69,1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="B70">
         <v>0</v>
       </c>
       <c r="D70">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="G70">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G70:G133" si="1">IF(B70=E70,1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B71">
         <v>0</v>
       </c>
       <c r="D71">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -2121,13 +2196,13 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>478</v>
+        <v>453</v>
       </c>
       <c r="B72">
         <v>0</v>
       </c>
       <c r="D72">
-        <v>478</v>
+        <v>453</v>
       </c>
       <c r="E72">
         <v>0</v>
@@ -2139,13 +2214,13 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>552</v>
+        <v>478</v>
       </c>
       <c r="B73">
         <v>0</v>
       </c>
       <c r="D73">
-        <v>552</v>
+        <v>478</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -2157,13 +2232,13 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="B74">
         <v>0</v>
       </c>
       <c r="D74">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -2175,13 +2250,13 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B75">
         <v>0</v>
       </c>
       <c r="D75">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -2193,13 +2268,13 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="B76">
         <v>0</v>
       </c>
       <c r="D76">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -2211,13 +2286,13 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
       <c r="D77">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -2229,13 +2304,13 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B78">
         <v>0</v>
       </c>
       <c r="D78">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -2247,13 +2322,13 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="B79">
         <v>0</v>
       </c>
       <c r="D79">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -2265,13 +2340,13 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B80">
         <v>0</v>
       </c>
       <c r="D80">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -2283,13 +2358,13 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>602</v>
+        <v>590</v>
       </c>
       <c r="B81">
         <v>0</v>
       </c>
       <c r="D81">
-        <v>602</v>
+        <v>590</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -2301,13 +2376,13 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>609</v>
+        <v>602</v>
       </c>
       <c r="B82">
         <v>0</v>
       </c>
       <c r="D82">
-        <v>609</v>
+        <v>602</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -2319,13 +2394,13 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>631</v>
+        <v>609</v>
       </c>
       <c r="B83">
         <v>0</v>
       </c>
       <c r="D83">
-        <v>631</v>
+        <v>609</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -2337,13 +2412,13 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>646</v>
+        <v>631</v>
       </c>
       <c r="B84">
         <v>0</v>
       </c>
       <c r="D84">
-        <v>646</v>
+        <v>631</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -2355,13 +2430,13 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="B85">
         <v>0</v>
       </c>
       <c r="D85">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="E85">
         <v>0</v>
@@ -2373,13 +2448,13 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="B86">
         <v>0</v>
       </c>
       <c r="D86">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="E86">
         <v>0</v>
@@ -2391,13 +2466,13 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>697</v>
+        <v>658</v>
       </c>
       <c r="B87">
         <v>0</v>
       </c>
       <c r="D87">
-        <v>697</v>
+        <v>658</v>
       </c>
       <c r="E87">
         <v>0</v>
@@ -2409,13 +2484,13 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B88">
         <v>0</v>
       </c>
       <c r="D88">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="E88">
         <v>0</v>
@@ -2427,13 +2502,13 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>720</v>
+        <v>699</v>
       </c>
       <c r="B89">
         <v>0</v>
       </c>
       <c r="D89">
-        <v>720</v>
+        <v>699</v>
       </c>
       <c r="E89">
         <v>0</v>
@@ -2445,13 +2520,13 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="B90">
         <v>0</v>
       </c>
       <c r="D90">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E90">
         <v>0</v>
@@ -2463,13 +2538,13 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="B91">
         <v>0</v>
       </c>
       <c r="D91">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="E91">
         <v>0</v>
@@ -2481,13 +2556,13 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B92">
         <v>0</v>
       </c>
       <c r="D92">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="E92">
         <v>0</v>
@@ -2499,13 +2574,13 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="B93">
         <v>0</v>
       </c>
       <c r="D93">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -2517,13 +2592,13 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="B94">
         <v>0</v>
       </c>
       <c r="D94">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="E94">
         <v>0</v>
@@ -2535,13 +2610,13 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B95">
         <v>0</v>
       </c>
       <c r="D95">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E95">
         <v>0</v>
@@ -2553,13 +2628,13 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="B96">
         <v>0</v>
       </c>
       <c r="D96">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="E96">
         <v>0</v>
@@ -2571,13 +2646,13 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>753</v>
+        <v>745</v>
       </c>
       <c r="B97">
         <v>0</v>
       </c>
       <c r="D97">
-        <v>753</v>
+        <v>745</v>
       </c>
       <c r="E97">
         <v>0</v>
@@ -2589,13 +2664,13 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="B98">
         <v>0</v>
       </c>
       <c r="D98">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="E98">
         <v>0</v>
@@ -2607,13 +2682,13 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="B99">
         <v>0</v>
       </c>
       <c r="D99">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="E99">
         <v>0</v>
@@ -2625,13 +2700,13 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="B100">
         <v>0</v>
       </c>
       <c r="D100">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E100">
         <v>0</v>
@@ -2643,13 +2718,13 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>775</v>
+        <v>766</v>
       </c>
       <c r="B101">
         <v>0</v>
       </c>
       <c r="D101">
-        <v>775</v>
+        <v>766</v>
       </c>
       <c r="E101">
         <v>0</v>
@@ -2661,13 +2736,13 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>787</v>
+        <v>775</v>
       </c>
       <c r="B102">
         <v>0</v>
       </c>
       <c r="D102">
-        <v>787</v>
+        <v>775</v>
       </c>
       <c r="E102">
         <v>0</v>
@@ -2679,13 +2754,13 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>795</v>
+        <v>787</v>
       </c>
       <c r="B103">
         <v>0</v>
       </c>
       <c r="D103">
-        <v>795</v>
+        <v>787</v>
       </c>
       <c r="E103">
         <v>0</v>
@@ -2697,13 +2772,13 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>810</v>
+        <v>795</v>
       </c>
       <c r="B104">
         <v>0</v>
       </c>
       <c r="D104">
-        <v>810</v>
+        <v>795</v>
       </c>
       <c r="E104">
         <v>0</v>
@@ -2715,13 +2790,13 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B105">
         <v>0</v>
       </c>
       <c r="D105">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E105">
         <v>0</v>
@@ -2733,13 +2808,13 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>818</v>
+        <v>811</v>
       </c>
       <c r="B106">
         <v>0</v>
       </c>
       <c r="D106">
-        <v>818</v>
+        <v>811</v>
       </c>
       <c r="E106">
         <v>0</v>
@@ -2751,13 +2826,13 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B107">
         <v>0</v>
       </c>
       <c r="D107">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="E107">
         <v>0</v>
@@ -2769,13 +2844,13 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>831</v>
+        <v>820</v>
       </c>
       <c r="B108">
         <v>0</v>
       </c>
       <c r="D108">
-        <v>831</v>
+        <v>820</v>
       </c>
       <c r="E108">
         <v>0</v>
@@ -2787,13 +2862,13 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B109">
         <v>0</v>
       </c>
       <c r="D109">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E109">
         <v>0</v>
@@ -2805,13 +2880,13 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B110">
         <v>0</v>
       </c>
       <c r="D110">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E110">
         <v>0</v>
@@ -2823,13 +2898,13 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>847</v>
+        <v>833</v>
       </c>
       <c r="B111">
         <v>0</v>
       </c>
       <c r="D111">
-        <v>847</v>
+        <v>833</v>
       </c>
       <c r="E111">
         <v>0</v>
@@ -2841,13 +2916,13 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>861</v>
+        <v>847</v>
       </c>
       <c r="B112">
         <v>0</v>
       </c>
       <c r="D112">
-        <v>861</v>
+        <v>847</v>
       </c>
       <c r="E112">
         <v>0</v>
@@ -2859,13 +2934,13 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>868</v>
+        <v>861</v>
       </c>
       <c r="B113">
         <v>0</v>
       </c>
       <c r="D113">
-        <v>868</v>
+        <v>861</v>
       </c>
       <c r="E113">
         <v>0</v>
@@ -2877,13 +2952,13 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>873</v>
+        <v>868</v>
       </c>
       <c r="B114">
         <v>0</v>
       </c>
       <c r="D114">
-        <v>873</v>
+        <v>868</v>
       </c>
       <c r="E114">
         <v>0</v>
@@ -2895,13 +2970,13 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>885</v>
+        <v>873</v>
       </c>
       <c r="B115">
         <v>0</v>
       </c>
       <c r="D115">
-        <v>885</v>
+        <v>873</v>
       </c>
       <c r="E115">
         <v>0</v>
@@ -2913,13 +2988,13 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>898</v>
+        <v>885</v>
       </c>
       <c r="B116">
         <v>0</v>
       </c>
       <c r="D116">
-        <v>898</v>
+        <v>885</v>
       </c>
       <c r="E116">
         <v>0</v>
@@ -2931,13 +3006,13 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>907</v>
+        <v>898</v>
       </c>
       <c r="B117">
         <v>0</v>
       </c>
       <c r="D117">
-        <v>907</v>
+        <v>898</v>
       </c>
       <c r="E117">
         <v>0</v>
@@ -2949,13 +3024,13 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>921</v>
+        <v>907</v>
       </c>
       <c r="B118">
         <v>0</v>
       </c>
       <c r="D118">
-        <v>921</v>
+        <v>907</v>
       </c>
       <c r="E118">
         <v>0</v>
@@ -2967,13 +3042,13 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>933</v>
+        <v>921</v>
       </c>
       <c r="B119">
         <v>0</v>
       </c>
       <c r="D119">
-        <v>933</v>
+        <v>921</v>
       </c>
       <c r="E119">
         <v>0</v>
@@ -2985,13 +3060,13 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>944</v>
+        <v>933</v>
       </c>
       <c r="B120">
         <v>0</v>
       </c>
       <c r="D120">
-        <v>944</v>
+        <v>933</v>
       </c>
       <c r="E120">
         <v>0</v>
@@ -3003,13 +3078,13 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>953</v>
+        <v>944</v>
       </c>
       <c r="B121">
         <v>0</v>
       </c>
       <c r="D121">
-        <v>953</v>
+        <v>944</v>
       </c>
       <c r="E121">
         <v>0</v>
@@ -3021,13 +3096,13 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>975</v>
+        <v>953</v>
       </c>
       <c r="B122">
         <v>0</v>
       </c>
       <c r="D122">
-        <v>975</v>
+        <v>953</v>
       </c>
       <c r="E122">
         <v>0</v>
@@ -3039,13 +3114,13 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>992</v>
+        <v>975</v>
       </c>
       <c r="B123">
         <v>0</v>
       </c>
       <c r="D123">
-        <v>992</v>
+        <v>975</v>
       </c>
       <c r="E123">
         <v>0</v>
@@ -3057,31 +3132,31 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>374</v>
+        <v>992</v>
       </c>
       <c r="B124">
         <v>0</v>
       </c>
       <c r="D124">
-        <v>374</v>
+        <v>992</v>
       </c>
       <c r="E124">
-        <v>1</v>
-      </c>
-      <c r="G124" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="G124">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="B125">
         <v>0</v>
       </c>
       <c r="D125">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="E125">
         <v>1</v>
@@ -3093,13 +3168,13 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B126">
         <v>0</v>
       </c>
       <c r="D126">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="E126">
         <v>1</v>
@@ -3111,13 +3186,13 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="B127">
         <v>0</v>
       </c>
       <c r="D127">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="E127">
         <v>1</v>
@@ -3129,13 +3204,13 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>422</v>
+        <v>400</v>
       </c>
       <c r="B128">
         <v>0</v>
       </c>
       <c r="D128">
-        <v>422</v>
+        <v>400</v>
       </c>
       <c r="E128">
         <v>1</v>
@@ -3147,13 +3222,13 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B129">
         <v>0</v>
       </c>
       <c r="D129">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E129">
         <v>1</v>
@@ -3165,13 +3240,13 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>444</v>
+        <v>426</v>
       </c>
       <c r="B130">
         <v>0</v>
       </c>
       <c r="D130">
-        <v>444</v>
+        <v>426</v>
       </c>
       <c r="E130">
         <v>1</v>
@@ -3183,13 +3258,13 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>486</v>
+        <v>444</v>
       </c>
       <c r="B131">
         <v>0</v>
       </c>
       <c r="D131">
-        <v>486</v>
+        <v>444</v>
       </c>
       <c r="E131">
         <v>1</v>
@@ -3201,13 +3276,13 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>540</v>
+        <v>486</v>
       </c>
       <c r="B132">
         <v>0</v>
       </c>
       <c r="D132">
-        <v>540</v>
+        <v>486</v>
       </c>
       <c r="E132">
         <v>1</v>
@@ -3219,49 +3294,49 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>551</v>
+        <v>540</v>
       </c>
       <c r="B133">
         <v>0</v>
       </c>
       <c r="D133">
-        <v>551</v>
+        <v>540</v>
       </c>
       <c r="E133">
         <v>1</v>
       </c>
       <c r="G133" t="b">
-        <f t="shared" ref="G133:G154" si="2">IF(B133=E133,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>591</v>
+        <v>551</v>
       </c>
       <c r="B134">
         <v>0</v>
       </c>
       <c r="D134">
-        <v>591</v>
+        <v>551</v>
       </c>
       <c r="E134">
         <v>1</v>
       </c>
       <c r="G134" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G134:G155" si="2">IF(B134=E134,1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>611</v>
+        <v>591</v>
       </c>
       <c r="B135">
         <v>0</v>
       </c>
       <c r="D135">
-        <v>611</v>
+        <v>591</v>
       </c>
       <c r="E135">
         <v>1</v>
@@ -3273,13 +3348,13 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="B136">
         <v>0</v>
       </c>
       <c r="D136">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="E136">
         <v>1</v>
@@ -3291,13 +3366,13 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="B137">
         <v>0</v>
       </c>
       <c r="D137">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="E137">
         <v>1</v>
@@ -3309,13 +3384,13 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B138">
         <v>0</v>
       </c>
       <c r="D138">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E138">
         <v>1</v>
@@ -3327,13 +3402,13 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>641</v>
+        <v>622</v>
       </c>
       <c r="B139">
         <v>0</v>
       </c>
       <c r="D139">
-        <v>641</v>
+        <v>622</v>
       </c>
       <c r="E139">
         <v>1</v>
@@ -3345,13 +3420,13 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>680</v>
+        <v>641</v>
       </c>
       <c r="B140">
         <v>0</v>
       </c>
       <c r="D140">
-        <v>680</v>
+        <v>641</v>
       </c>
       <c r="E140">
         <v>1</v>
@@ -3363,13 +3438,13 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>691</v>
+        <v>680</v>
       </c>
       <c r="B141">
         <v>0</v>
       </c>
       <c r="D141">
-        <v>691</v>
+        <v>680</v>
       </c>
       <c r="E141">
         <v>1</v>
@@ -3381,13 +3456,13 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>701</v>
+        <v>691</v>
       </c>
       <c r="B142">
         <v>0</v>
       </c>
       <c r="D142">
-        <v>701</v>
+        <v>691</v>
       </c>
       <c r="E142">
         <v>1</v>
@@ -3399,13 +3474,13 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B143">
         <v>0</v>
       </c>
       <c r="D143">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E143">
         <v>1</v>
@@ -3417,13 +3492,13 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>717</v>
+        <v>702</v>
       </c>
       <c r="B144">
         <v>0</v>
       </c>
       <c r="D144">
-        <v>717</v>
+        <v>702</v>
       </c>
       <c r="E144">
         <v>1</v>
@@ -3435,13 +3510,13 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>736</v>
+        <v>717</v>
       </c>
       <c r="B145">
         <v>0</v>
       </c>
       <c r="D145">
-        <v>736</v>
+        <v>717</v>
       </c>
       <c r="E145">
         <v>1</v>
@@ -3453,13 +3528,13 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>797</v>
+        <v>736</v>
       </c>
       <c r="B146">
         <v>0</v>
       </c>
       <c r="D146">
-        <v>797</v>
+        <v>736</v>
       </c>
       <c r="E146">
         <v>1</v>
@@ -3471,13 +3546,13 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B147">
         <v>0</v>
       </c>
       <c r="D147">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="E147">
         <v>1</v>
@@ -3489,13 +3564,13 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="B148">
         <v>0</v>
       </c>
       <c r="D148">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="E148">
         <v>1</v>
@@ -3507,13 +3582,13 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>834</v>
+        <v>803</v>
       </c>
       <c r="B149">
         <v>0</v>
       </c>
       <c r="D149">
-        <v>834</v>
+        <v>803</v>
       </c>
       <c r="E149">
         <v>1</v>
@@ -3525,13 +3600,13 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>850</v>
+        <v>834</v>
       </c>
       <c r="B150">
         <v>0</v>
       </c>
       <c r="D150">
-        <v>850</v>
+        <v>834</v>
       </c>
       <c r="E150">
         <v>1</v>
@@ -3543,13 +3618,13 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="B151">
         <v>0</v>
       </c>
       <c r="D151">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="E151">
         <v>1</v>
@@ -3561,13 +3636,13 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="B152">
         <v>0</v>
       </c>
       <c r="D152">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="E152">
         <v>1</v>
@@ -3579,13 +3654,13 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>877</v>
+        <v>856</v>
       </c>
       <c r="B153">
         <v>0</v>
       </c>
       <c r="D153">
-        <v>877</v>
+        <v>856</v>
       </c>
       <c r="E153">
         <v>1</v>
@@ -3597,13 +3672,13 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B154">
         <v>0</v>
       </c>
       <c r="D154">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="E154">
         <v>1</v>
@@ -3613,13 +3688,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G156">
-        <f>SUM(G4:G155)/151</f>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>878</v>
+      </c>
+      <c r="B155">
+        <v>0</v>
+      </c>
+      <c r="D155">
+        <v>878</v>
+      </c>
+      <c r="E155">
+        <v>1</v>
+      </c>
+      <c r="G155" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G157">
+        <f>SUM(G5:G156)/151</f>
         <v>0.79470198675496684</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>